<commit_message>
Remove errant space from test data
</commit_message>
<xml_diff>
--- a/tests/bin/COUNTER_workbooks_for_tests/2_2019.xlsx
+++ b/tests/bin/COUNTER_workbooks_for_tests/2_2019.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -929,15 +929,12 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>

</xml_diff>